<commit_message>
Ind MF - Added indexes
</commit_message>
<xml_diff>
--- a/Reports/IndMFData/IndMF_Index.xlsx
+++ b/Reports/IndMFData/IndMF_Index.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i852841/_Codes/_Personal/StockRankingCrawler/Reports/IndMFData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6C8484A6-307C-3347-8D4C-DEE146CB055B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE9CF90-6187-D34A-9A67-8016023A5868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="19380" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NAV" r:id="rId1" sheetId="1"/>
-    <sheet name="UNDERLYINGINDEX" r:id="rId2" sheetId="2"/>
-    <sheet name="AUM" r:id="rId3" sheetId="3"/>
-    <sheet name="EXPENSERATIO" r:id="rId4" sheetId="4"/>
-    <sheet name="MANAGER" r:id="rId5" sheetId="5"/>
-    <sheet name="PERATIO" r:id="rId6" sheetId="6"/>
-    <sheet name="PBRATIO" r:id="rId7" sheetId="7"/>
-    <sheet name="52Week" r:id="rId8" sheetId="8"/>
+    <sheet name="NAV" sheetId="1" r:id="rId1"/>
+    <sheet name="UNDERLYINGINDEX" sheetId="2" r:id="rId2"/>
+    <sheet name="AUM" sheetId="3" r:id="rId3"/>
+    <sheet name="EXPENSERATIO" sheetId="4" r:id="rId4"/>
+    <sheet name="MANAGER" sheetId="5" r:id="rId5"/>
+    <sheet name="PERATIO" sheetId="6" r:id="rId6"/>
+    <sheet name="PBRATIO" sheetId="7" r:id="rId7"/>
+    <sheet name="52Week" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="256">
   <si>
     <t>HDFC</t>
   </si>
@@ -732,23 +732,103 @@
     <t>4.03---4.1</t>
   </si>
   <si>
-    <t>N250</t>
-  </si>
-  <si>
-    <t>N50</t>
-  </si>
-  <si>
-    <t/>
+    <t>NIFTY Smallcap 100</t>
+  </si>
+  <si>
+    <t>Nifty Smallcap 250</t>
+  </si>
+  <si>
+    <t>BSE 250 Smallcap</t>
+  </si>
+  <si>
+    <t>BSE SmallCap</t>
+  </si>
+  <si>
+    <t>BSE 400 MidSmallCap</t>
+  </si>
+  <si>
+    <t>Nifty Midcap 50</t>
+  </si>
+  <si>
+    <t>NIFTY Midcap 100</t>
+  </si>
+  <si>
+    <t>BSE 150 Midcap</t>
+  </si>
+  <si>
+    <t>Nifty 50</t>
+  </si>
+  <si>
+    <t>Nifty 500</t>
+  </si>
+  <si>
+    <t>BSE Sensex</t>
+  </si>
+  <si>
+    <t>BSE Sensex 50</t>
+  </si>
+  <si>
+    <t>BSE India Manufacturing</t>
+  </si>
+  <si>
+    <t>BSE Sensex Next 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India VIX </t>
   </si>
   <si>
     <t>Nov_30</t>
+  </si>
+  <si>
+    <t>5,814.85</t>
+  </si>
+  <si>
+    <t>4,831.05</t>
+  </si>
+  <si>
+    <t>13,560.57</t>
+  </si>
+  <si>
+    <t>2,010.97</t>
+  </si>
+  <si>
+    <t>3,574.38</t>
+  </si>
+  <si>
+    <t>4,722.80</t>
+  </si>
+  <si>
+    <t>17,222.15</t>
+  </si>
+  <si>
+    <t>4,761.78</t>
+  </si>
+  <si>
+    <t>12,056.05</t>
+  </si>
+  <si>
+    <t>9,813.65</t>
+  </si>
+  <si>
+    <t>40,793.81</t>
+  </si>
+  <si>
+    <t>12,605.82</t>
+  </si>
+  <si>
+    <t>31,825.59</t>
+  </si>
+  <si>
+    <t>459.30</t>
+  </si>
+  <si>
+    <t>13.8975</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -758,22 +838,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="45"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="45"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -786,353 +856,351 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="338">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="10" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+  <cellXfs count="336">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1149,10 +1217,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1187,7 +1255,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1239,7 +1307,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1350,21 +1418,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1381,7 +1449,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1433,64 +1501,159 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="7.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="7.6640625" collapsed="false"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C1" s="93" t="s">
-        <v>20</v>
+      <c r="B1" s="335" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="93" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="336" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" s="93" t="n">
-        <v>1.0</v>
+      <c r="B2" s="335" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="93" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="337" t="s">
+      <c r="B3" s="335" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="335" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" s="335" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="335" t="s">
         <v>227</v>
       </c>
-      <c r="C3" s="93" t="n">
-        <v>2.0</v>
+      <c r="B5" s="335" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="335" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="335" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="335" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="335" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" s="335" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="335" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="335" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="335" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="335" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="335" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B15" s="335" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>239</v>
+      </c>
+      <c r="B16" s="335" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E10517-3041-A548-8327-A322F0969D22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E10517-3041-A548-8327-A322F0969D22}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1499,9 +1662,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1755,12 +1918,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31A2CC3-117B-3044-9A40-45E232EE90D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31A2CC3-117B-3044-9A40-45E232EE90D3}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1769,9 +1932,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="11.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2025,12 +2188,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7F83E3-8D7E-E84F-B4A5-9AABCBB25C75}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7F83E3-8D7E-E84F-B4A5-9AABCBB25C75}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2039,10 +2202,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="7.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.83203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2365,12 +2528,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1FCE02-3D0C-1545-8192-6E055D0C99D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1FCE02-3D0C-1545-8192-6E055D0C99D5}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2379,10 +2542,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="19.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2705,12 +2868,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6044C64-1C8D-2144-BC85-693CF5996D95}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6044C64-1C8D-2144-BC85-693CF5996D95}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2719,10 +2882,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="11.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3045,12 +3208,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311CB058-A4EB-6F43-B724-C153741DCABC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311CB058-A4EB-6F43-B724-C153741DCABC}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3059,10 +3222,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="31.83203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="31.83203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.83203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3385,22 +3548,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E466B42B-1FD8-C746-8F67-0DBD703B7828}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E466B42B-1FD8-C746-8F67-0DBD703B7828}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="140" zoomScaleNormal="140">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -3586,6 +3749,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>